<commit_message>
ITkl8JTn [Translated every single russian word to english. Suppressed exception inspection] Created Trait, tests and docker configuration
</commit_message>
<xml_diff>
--- a/tests/xlsxFiles/example.xlsx
+++ b/tests/xlsxFiles/example.xlsx
@@ -15,40 +15,49 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">смешанный </t>
+      <t xml:space="preserve">mixed </t>
     </r>
     <r>
-      <t>шрифт</t>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>font</t>
     </r>
   </si>
   <si>
-    <t>зелёный</t>
-  </si>
-  <si>
-    <t>горизонтальное центрирование</t>
-  </si>
-  <si>
-    <t>обтекание текста вокруг границ</t>
-  </si>
-  <si>
-    <t>нормальный шрифт</t>
-  </si>
-  <si>
-    <t>красный</t>
-  </si>
-  <si>
-    <t>вертикальное центрирование</t>
-  </si>
-  <si>
-    <t>ширина 14.43</t>
-  </si>
-  <si>
-    <t>жёлтый</t>
-  </si>
-  <si>
-    <t>ширина 57.29</t>
+    <t>green</t>
+  </si>
+  <si>
+    <t>horizontal alignment</t>
+  </si>
+  <si>
+    <t>wrap text</t>
+  </si>
+  <si>
+    <t>regular font</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>vertical alignment</t>
+  </si>
+  <si>
+    <t>width 14.43</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>width 57.29</t>
   </si>
 </sst>
 </file>
@@ -62,24 +71,34 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF00FF00"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF34A853"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="5"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FFFBBC04"/>
+      <sz val="11.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FFFFFF00"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -97,42 +116,51 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -163,40 +191,40 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -343,19 +371,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.14"/>
+    <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="57.29"/>
     <col customWidth="1" min="4" max="4" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,28 +399,31 @@
       </c>
     </row>
     <row r="2" ht="35.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" ht="26.25" customHeight="1">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>